<commit_message>
benchmark - PhageDPO & DePP results
</commit_message>
<xml_diff>
--- a/data/Benchmarking/benchmark_depos_results.xlsx
+++ b/data/Benchmarking/benchmark_depos_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimi/Documents/GitHub/PhageDEPOdetection/data/Benchmarking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93BAB25D-E315-2449-BC37-C81D155C8B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEE93FC-7B5C-A248-9CDD-0715D12409F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1000" windowWidth="27840" windowHeight="15900" xr2:uid="{3161CBD2-B915-5A4B-B858-6DF04D2DDE0F}"/>
+    <workbookView xWindow="-33600" yWindow="-2500" windowWidth="27840" windowHeight="15900" xr2:uid="{3161CBD2-B915-5A4B-B858-6DF04D2DDE0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t>Table XX: benchmarking results of PhageDPO, DePP and PhageDEPOdetection on the Pires 2016 dataset</t>
   </si>
@@ -459,14 +459,37 @@
   </si>
   <si>
     <t>NC_017972.1</t>
+  </si>
+  <si>
+    <t>PhageDPO predictions</t>
+  </si>
+  <si>
+    <t>DePP predictions</t>
+  </si>
+  <si>
+    <t>PhageDEPOdetection predictions</t>
+  </si>
+  <si>
+    <t>True positives (Pires)</t>
+  </si>
+  <si>
+    <t>We will need both the true positives but also the rue negatives.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -498,6 +521,14 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -525,18 +556,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -855,913 +890,932 @@
   <dimension ref="A1:P156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="P1" s="5"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="P1" s="6"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P2" s="5"/>
+      <c r="P2" s="6"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="5"/>
+      <c r="B3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="P3" s="6"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="P4" s="5"/>
+      <c r="P4" s="6"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="P5" s="5"/>
+      <c r="D5" t="s">
+        <v>145</v>
+      </c>
+      <c r="P5" s="6"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="P6" s="5"/>
+      <c r="P6" s="6"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="P7" s="5"/>
+      <c r="P7" s="6"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="P8" s="5"/>
+      <c r="P8" s="6"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="P9" s="5"/>
+      <c r="P9" s="6"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="P10" s="5"/>
+      <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="P11" s="5"/>
+      <c r="P11" s="6"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="P12" s="5"/>
+      <c r="P12" s="6"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="P13" s="5"/>
+      <c r="P13" s="6"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="P14" s="5"/>
+      <c r="P14" s="6"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="P15" s="5"/>
+      <c r="P15" s="6"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="P16" s="5"/>
+      <c r="P16" s="6"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P17" s="5"/>
+      <c r="P17" s="6"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="P18" s="5"/>
+      <c r="P18" s="6"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="P19" s="5"/>
+      <c r="P19" s="6"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="P20" s="5"/>
+      <c r="P20" s="6"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="P21" s="5"/>
+      <c r="P21" s="6"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="P22" s="5"/>
+      <c r="P22" s="6"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="P23" s="5"/>
+      <c r="P23" s="6"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="P24" s="5"/>
+      <c r="P24" s="6"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="P25" s="5"/>
+      <c r="P25" s="6"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="P26" s="5"/>
+      <c r="P26" s="6"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="P27" s="5"/>
+      <c r="P27" s="6"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="P28" s="5"/>
+      <c r="P28" s="6"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="P29" s="5"/>
+      <c r="P29" s="6"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P30" s="5"/>
+      <c r="P30" s="6"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="P31" s="5"/>
+      <c r="P31" s="6"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="P32" s="5"/>
+      <c r="P32" s="6"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="P33" s="4"/>
+      <c r="P33" s="5"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P34" s="4"/>
+      <c r="P34" s="5"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="P35" s="5"/>
+      <c r="P35" s="6"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P36" s="5"/>
+      <c r="P36" s="6"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="P37" s="5"/>
+      <c r="P37" s="6"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="P38" s="5"/>
+      <c r="P38" s="6"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="P39" s="5"/>
+      <c r="P39" s="6"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="P40" s="5"/>
+      <c r="P40" s="6"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P41" s="5"/>
+      <c r="P41" s="6"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="P42" s="5"/>
+      <c r="P42" s="6"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="P43" s="5"/>
+      <c r="P43" s="6"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="P44" s="5"/>
+      <c r="P44" s="6"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="P45" s="5"/>
+      <c r="P45" s="6"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="P46" s="5"/>
+      <c r="P46" s="6"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="P47" s="5"/>
+      <c r="P47" s="6"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P48" s="5"/>
+      <c r="P48" s="6"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P49" s="5"/>
+      <c r="P49" s="6"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="P50" s="5"/>
+      <c r="P50" s="6"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="P51" s="5"/>
+      <c r="P51" s="6"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="P52" s="5"/>
+      <c r="P52" s="6"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="P53" s="5"/>
+      <c r="P53" s="6"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P54" s="5"/>
+      <c r="P54" s="6"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P55" s="5"/>
+      <c r="P55" s="6"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="P56" s="5"/>
+      <c r="P56" s="6"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="P57" s="5"/>
+      <c r="P57" s="6"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="P58" s="5"/>
+      <c r="P58" s="6"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="P59" s="5"/>
+      <c r="P59" s="6"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="P60" s="5"/>
+      <c r="P60" s="6"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="P61" s="5"/>
+      <c r="P61" s="6"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="P62" s="5"/>
+      <c r="P62" s="6"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="P63" s="5"/>
+      <c r="P63" s="6"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="P64" s="5"/>
+      <c r="P64" s="6"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P65" s="5"/>
+      <c r="P65" s="6"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="P66" s="5"/>
+      <c r="P66" s="6"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="P67" s="5"/>
+      <c r="P67" s="6"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="P68" s="5"/>
+      <c r="P68" s="6"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P69" s="5"/>
+      <c r="P69" s="6"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="P70" s="5"/>
+      <c r="P70" s="6"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
+      <c r="A71" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="P71" s="5"/>
+      <c r="P71" s="6"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="P72" s="5"/>
+      <c r="P72" s="6"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="P73" s="5"/>
+      <c r="P73" s="6"/>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="P74" s="5"/>
+      <c r="P74" s="6"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
+      <c r="A75" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="P75" s="5"/>
+      <c r="P75" s="6"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="P76" s="5"/>
+      <c r="P76" s="6"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A77" s="5" t="s">
+      <c r="A77" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="P77" s="5"/>
+      <c r="P77" s="6"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="P78" s="5"/>
+      <c r="P78" s="6"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="P79" s="5"/>
+      <c r="P79" s="6"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="P80" s="4"/>
+      <c r="P80" s="5"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="P81" s="4"/>
+      <c r="P81" s="5"/>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P82" s="5"/>
+      <c r="P82" s="6"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A83" s="5" t="s">
+      <c r="A83" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="P83" s="5"/>
+      <c r="P83" s="6"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="P84" s="5"/>
+      <c r="P84" s="6"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="P85" s="5"/>
+      <c r="P85" s="6"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="P86" s="5"/>
+      <c r="P86" s="6"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="P87" s="5"/>
+      <c r="P87" s="6"/>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="P88" s="5"/>
+      <c r="P88" s="6"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="P89" s="5"/>
+      <c r="P89" s="6"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="P90" s="5"/>
+      <c r="P90" s="6"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A91" s="4" t="s">
+      <c r="A91" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="P91" s="5"/>
+      <c r="P91" s="6"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="P92" s="5"/>
+      <c r="P92" s="6"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="P93" s="4"/>
+      <c r="P93" s="5"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="P94" s="4"/>
+      <c r="P94" s="5"/>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="P95" s="4"/>
+      <c r="P95" s="5"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A96" s="5" t="s">
+      <c r="A96" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P96" s="4"/>
+      <c r="P96" s="5"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="P97" s="4"/>
+      <c r="P97" s="5"/>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A98" s="5" t="s">
+      <c r="A98" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="P98" s="5"/>
+      <c r="P98" s="6"/>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A99" s="5" t="s">
+      <c r="A99" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="P99" s="5"/>
+      <c r="P99" s="6"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A100" s="5" t="s">
+      <c r="A100" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="P100" s="5"/>
+      <c r="P100" s="6"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A101" s="5" t="s">
+      <c r="A101" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="P101" s="5"/>
+      <c r="P101" s="6"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A102" s="5" t="s">
+      <c r="A102" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P102" s="5"/>
+      <c r="P102" s="6"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A103" s="5" t="s">
+      <c r="A103" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="P103" s="5"/>
+      <c r="P103" s="6"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A104" s="4" t="s">
+      <c r="A104" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="P104" s="5"/>
+      <c r="P104" s="6"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A105" s="5" t="s">
+      <c r="A105" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="P105" s="5"/>
+      <c r="P105" s="6"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A106" s="4" t="s">
+      <c r="A106" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="P106" s="5"/>
+      <c r="P106" s="6"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A107" s="5" t="s">
+      <c r="A107" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="P107" s="5"/>
+      <c r="P107" s="6"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A108" s="5" t="s">
+      <c r="A108" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="P108" s="5"/>
+      <c r="P108" s="6"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A109" s="5" t="s">
+      <c r="A109" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="P109" s="5"/>
+      <c r="P109" s="6"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A110" s="5" t="s">
+      <c r="A110" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="P110" s="4"/>
+      <c r="P110" s="5"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A111" s="5" t="s">
+      <c r="A111" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="P111" s="4"/>
+      <c r="P111" s="5"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A112" s="5" t="s">
+      <c r="A112" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="P112" s="5"/>
+      <c r="P112" s="6"/>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A113" s="5" t="s">
+      <c r="A113" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="P113" s="4"/>
+      <c r="P113" s="5"/>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A114" s="4" t="s">
+      <c r="A114" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="P114" s="4"/>
+      <c r="P114" s="5"/>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A115" s="5" t="s">
+      <c r="A115" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="P115" s="4"/>
+      <c r="P115" s="5"/>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A116" s="5" t="s">
+      <c r="A116" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="P116" s="4"/>
+      <c r="P116" s="5"/>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A117" s="5" t="s">
+      <c r="A117" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="P117" s="5"/>
+      <c r="P117" s="6"/>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A118" s="5" t="s">
+      <c r="A118" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="P118" s="5"/>
+      <c r="P118" s="6"/>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A119" s="5" t="s">
+      <c r="A119" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="P119" s="5"/>
+      <c r="P119" s="6"/>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A120" s="5" t="s">
+      <c r="A120" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="P120" s="5"/>
+      <c r="P120" s="6"/>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A121" s="5" t="s">
+      <c r="A121" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="P121" s="5"/>
+      <c r="P121" s="6"/>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A122" s="5" t="s">
+      <c r="A122" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="P122" s="5"/>
+      <c r="P122" s="6"/>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A123" s="5" t="s">
+      <c r="A123" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="P123" s="5"/>
+      <c r="P123" s="6"/>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A124" s="5" t="s">
+      <c r="A124" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="P124" s="4"/>
+      <c r="P124" s="5"/>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A125" s="5" t="s">
+      <c r="A125" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="P125" s="4"/>
+      <c r="P125" s="5"/>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A126" s="5" t="s">
+      <c r="A126" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="P126" s="5"/>
+      <c r="P126" s="6"/>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A127" s="5" t="s">
+      <c r="A127" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="P127" s="5"/>
+      <c r="P127" s="6"/>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A128" s="5" t="s">
+      <c r="A128" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="P128" s="5"/>
+      <c r="P128" s="6"/>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A129" s="5" t="s">
+      <c r="A129" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="P129" s="5"/>
+      <c r="P129" s="6"/>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A130" s="5" t="s">
+      <c r="A130" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="P130" s="5"/>
+      <c r="P130" s="6"/>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A131" s="5" t="s">
+      <c r="A131" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="P131" s="5"/>
+      <c r="P131" s="6"/>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A132" s="5" t="s">
+      <c r="A132" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="P132" s="5"/>
+      <c r="P132" s="6"/>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A133" s="5" t="s">
+      <c r="A133" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="P133" s="5"/>
+      <c r="P133" s="6"/>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A134" s="5" t="s">
+      <c r="A134" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="P134" s="5"/>
+      <c r="P134" s="6"/>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A135" s="5" t="s">
+      <c r="A135" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="P135" s="5"/>
+      <c r="P135" s="6"/>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A136" s="5" t="s">
+      <c r="A136" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P136" s="5"/>
+      <c r="P136" s="6"/>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A137" s="5" t="s">
+      <c r="A137" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P137" s="5"/>
+      <c r="P137" s="6"/>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A138" s="5" t="s">
+      <c r="A138" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="P138" s="5"/>
+      <c r="P138" s="6"/>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A139" s="5" t="s">
+      <c r="A139" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P139" s="5"/>
+      <c r="P139" s="6"/>
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A140" s="5" t="s">
+      <c r="A140" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="P140" s="5"/>
+      <c r="P140" s="6"/>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A141" s="4" t="s">
+      <c r="A141" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P141" s="5"/>
+      <c r="P141" s="6"/>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A142" s="5" t="s">
+      <c r="A142" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="P142" s="5"/>
+      <c r="P142" s="6"/>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P143" s="5"/>
+      <c r="P143" s="6"/>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P144" s="5"/>
+      <c r="P144" s="6"/>
     </row>
     <row r="145" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P145" s="5"/>
+      <c r="P145" s="6"/>
     </row>
     <row r="146" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P146" s="5"/>
+      <c r="P146" s="6"/>
     </row>
     <row r="147" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P147" s="5"/>
+      <c r="P147" s="6"/>
     </row>
     <row r="148" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P148" s="5"/>
+      <c r="P148" s="6"/>
     </row>
     <row r="149" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P149" s="5"/>
+      <c r="P149" s="6"/>
     </row>
     <row r="150" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P150" s="5"/>
+      <c r="P150" s="6"/>
     </row>
     <row r="151" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P151" s="5"/>
+      <c r="P151" s="6"/>
     </row>
     <row r="152" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P152" s="5"/>
+      <c r="P152" s="6"/>
     </row>
     <row r="153" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P153" s="4"/>
+      <c r="P153" s="5"/>
     </row>
     <row r="154" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P154" s="4"/>
+      <c r="P154" s="5"/>
     </row>
     <row r="155" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P155" s="5"/>
+      <c r="P155" s="6"/>
     </row>
     <row r="156" spans="16:16" x14ac:dyDescent="0.2">
-      <c r="P156" s="3"/>
+      <c r="P156" s="4"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P1:P158">

</xml_diff>